<commit_message>
Add categorical summary stats
</commit_message>
<xml_diff>
--- a/output/residue_extraction/OleA_machine_learning_results_categorical.xlsx
+++ b/output/residue_extraction/OleA_machine_learning_results_categorical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aed3d806ed7068fe/Documents/GitHub/TARA-thiolases/output/residue_extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{4B838C9B-D726-4C25-B1C7-1E7BC57797C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6C156EBE-14F0-407F-A7D4-B191E6340488}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{4B838C9B-D726-4C25-B1C7-1E7BC57797C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{18D8F020-08C6-4895-8E64-FBFF1B2BCEAE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CA3EB40E-2DA2-4F94-A8D8-F0FF99F49B04}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="12">
   <si>
     <t>feature_set</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>tt_split</t>
-  </si>
-  <si>
-    <t>threshhold</t>
   </si>
   <si>
     <t>oob_error</t>
@@ -66,6 +63,12 @@
   </si>
   <si>
     <t>20, 30</t>
+  </si>
+  <si>
+    <t>15, 30</t>
+  </si>
+  <si>
+    <t>threshold</t>
   </si>
 </sst>
 </file>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB5DCEB-1489-4786-BE72-895616BF0A17}">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,30 +450,30 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0.7</v>
@@ -499,7 +502,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>0.7</v>
@@ -528,7 +531,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0.7</v>
@@ -557,7 +560,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0.7</v>
@@ -586,7 +589,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0.7</v>
@@ -615,7 +618,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0.7</v>
@@ -644,7 +647,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>0.7</v>
@@ -673,7 +676,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0.7</v>
@@ -702,7 +705,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0.7</v>
@@ -731,7 +734,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>0.7</v>
@@ -760,7 +763,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>0.8</v>
@@ -789,7 +792,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>0.8</v>
@@ -818,7 +821,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>0.8</v>
@@ -847,7 +850,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <v>0.8</v>
@@ -876,7 +879,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>0.8</v>
@@ -905,7 +908,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>0.8</v>
@@ -934,7 +937,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>0.8</v>
@@ -963,7 +966,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>0.8</v>
@@ -992,7 +995,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>0.8</v>
@@ -1021,7 +1024,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21">
         <v>0.8</v>
@@ -1050,7 +1053,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22">
         <v>0.7</v>
@@ -1079,7 +1082,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23">
         <v>0.7</v>
@@ -1108,7 +1111,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24">
         <v>0.7</v>
@@ -1137,7 +1140,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>0.7</v>
@@ -1166,7 +1169,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26">
         <v>0.7</v>
@@ -1195,7 +1198,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27">
         <v>0.7</v>
@@ -1224,7 +1227,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28">
         <v>0.7</v>
@@ -1253,7 +1256,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29">
         <v>0.7</v>
@@ -1282,7 +1285,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30">
         <v>0.7</v>
@@ -1311,7 +1314,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31">
         <v>0.7</v>
@@ -1340,7 +1343,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32">
         <v>0.8</v>
@@ -1369,7 +1372,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33">
         <v>0.8</v>
@@ -1398,7 +1401,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34">
         <v>0.8</v>
@@ -1427,7 +1430,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35">
         <v>0.8</v>
@@ -1456,7 +1459,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36">
         <v>0.8</v>
@@ -1485,7 +1488,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37">
         <v>0.8</v>
@@ -1514,7 +1517,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38">
         <v>0.8</v>
@@ -1543,7 +1546,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39">
         <v>0.8</v>
@@ -1572,7 +1575,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B40">
         <v>0.8</v>
@@ -1601,7 +1604,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41">
         <v>0.8</v>
@@ -1630,7 +1633,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B42">
         <v>0.7</v>
@@ -1642,7 +1645,7 @@
         <v>3</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1659,7 +1662,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B43">
         <v>0.7</v>
@@ -1671,7 +1674,7 @@
         <v>3</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43">
         <v>2</v>
@@ -1688,7 +1691,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B44">
         <v>0.7</v>
@@ -1700,7 +1703,7 @@
         <v>3</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44">
         <v>3</v>
@@ -1717,7 +1720,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45">
         <v>0.7</v>
@@ -1729,7 +1732,7 @@
         <v>3</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45">
         <v>4</v>
@@ -1746,7 +1749,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B46">
         <v>0.7</v>
@@ -1758,7 +1761,7 @@
         <v>3</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F46">
         <v>5</v>
@@ -1775,7 +1778,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47">
         <v>0.7</v>
@@ -1787,7 +1790,7 @@
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47">
         <v>6</v>
@@ -1804,7 +1807,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48">
         <v>0.7</v>
@@ -1816,7 +1819,7 @@
         <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F48">
         <v>7</v>
@@ -1833,7 +1836,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B49">
         <v>0.7</v>
@@ -1845,7 +1848,7 @@
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F49">
         <v>8</v>
@@ -1862,7 +1865,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B50">
         <v>0.7</v>
@@ -1874,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="E50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50">
         <v>9</v>
@@ -1891,7 +1894,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B51">
         <v>0.7</v>
@@ -1903,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51">
         <v>10</v>
@@ -1920,7 +1923,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52">
         <v>0.8</v>
@@ -1932,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -1949,7 +1952,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B53">
         <v>0.8</v>
@@ -1961,7 +1964,7 @@
         <v>3</v>
       </c>
       <c r="E53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53">
         <v>2</v>
@@ -1978,7 +1981,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B54">
         <v>0.8</v>
@@ -1990,7 +1993,7 @@
         <v>3</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54">
         <v>3</v>
@@ -2007,7 +2010,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B55">
         <v>0.8</v>
@@ -2019,7 +2022,7 @@
         <v>3</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55">
         <v>4</v>
@@ -2036,7 +2039,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56">
         <v>0.8</v>
@@ -2048,7 +2051,7 @@
         <v>3</v>
       </c>
       <c r="E56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56">
         <v>5</v>
@@ -2065,7 +2068,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57">
         <v>0.8</v>
@@ -2077,7 +2080,7 @@
         <v>3</v>
       </c>
       <c r="E57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57">
         <v>6</v>
@@ -2094,7 +2097,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B58">
         <v>0.8</v>
@@ -2106,7 +2109,7 @@
         <v>3</v>
       </c>
       <c r="E58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58">
         <v>7</v>
@@ -2123,7 +2126,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B59">
         <v>0.8</v>
@@ -2135,7 +2138,7 @@
         <v>3</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59">
         <v>8</v>
@@ -2152,7 +2155,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B60">
         <v>0.8</v>
@@ -2164,7 +2167,7 @@
         <v>3</v>
       </c>
       <c r="E60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60">
         <v>9</v>
@@ -2181,7 +2184,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B61">
         <v>0.8</v>
@@ -2193,7 +2196,7 @@
         <v>3</v>
       </c>
       <c r="E61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F61">
         <v>10</v>
@@ -2210,7 +2213,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B62">
         <v>0.7</v>
@@ -2222,7 +2225,7 @@
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2239,7 +2242,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B63">
         <v>0.7</v>
@@ -2251,7 +2254,7 @@
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63">
         <v>2</v>
@@ -2268,7 +2271,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B64">
         <v>0.7</v>
@@ -2280,7 +2283,7 @@
         <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64">
         <v>3</v>
@@ -2297,7 +2300,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B65">
         <v>0.7</v>
@@ -2309,7 +2312,7 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65">
         <v>4</v>
@@ -2326,7 +2329,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B66">
         <v>0.7</v>
@@ -2338,7 +2341,7 @@
         <v>2</v>
       </c>
       <c r="E66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66">
         <v>5</v>
@@ -2355,7 +2358,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B67">
         <v>0.7</v>
@@ -2367,7 +2370,7 @@
         <v>2</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67">
         <v>6</v>
@@ -2384,7 +2387,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B68">
         <v>0.7</v>
@@ -2396,7 +2399,7 @@
         <v>2</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68">
         <v>7</v>
@@ -2413,7 +2416,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B69">
         <v>0.7</v>
@@ -2425,7 +2428,7 @@
         <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69">
         <v>8</v>
@@ -2442,7 +2445,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B70">
         <v>0.7</v>
@@ -2454,7 +2457,7 @@
         <v>2</v>
       </c>
       <c r="E70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70">
         <v>9</v>
@@ -2471,7 +2474,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B71">
         <v>0.7</v>
@@ -2483,7 +2486,7 @@
         <v>2</v>
       </c>
       <c r="E71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71">
         <v>10</v>
@@ -2500,7 +2503,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B72">
         <v>0.8</v>
@@ -2512,7 +2515,7 @@
         <v>2</v>
       </c>
       <c r="E72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2529,7 +2532,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B73">
         <v>0.8</v>
@@ -2541,7 +2544,7 @@
         <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73">
         <v>2</v>
@@ -2558,7 +2561,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B74">
         <v>0.8</v>
@@ -2570,7 +2573,7 @@
         <v>2</v>
       </c>
       <c r="E74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74">
         <v>3</v>
@@ -2587,7 +2590,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B75">
         <v>0.8</v>
@@ -2599,7 +2602,7 @@
         <v>2</v>
       </c>
       <c r="E75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75">
         <v>4</v>
@@ -2616,7 +2619,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B76">
         <v>0.8</v>
@@ -2628,7 +2631,7 @@
         <v>2</v>
       </c>
       <c r="E76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76">
         <v>5</v>
@@ -2645,7 +2648,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B77">
         <v>0.8</v>
@@ -2657,7 +2660,7 @@
         <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77">
         <v>6</v>
@@ -2674,7 +2677,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B78">
         <v>0.8</v>
@@ -2686,7 +2689,7 @@
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78">
         <v>7</v>
@@ -2703,7 +2706,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B79">
         <v>0.8</v>
@@ -2715,7 +2718,7 @@
         <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79">
         <v>8</v>
@@ -2732,7 +2735,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B80">
         <v>0.8</v>
@@ -2744,7 +2747,7 @@
         <v>2</v>
       </c>
       <c r="E80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80">
         <v>9</v>
@@ -2761,7 +2764,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B81">
         <v>0.8</v>
@@ -2773,7 +2776,7 @@
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81">
         <v>10</v>
@@ -2786,6 +2789,1166 @@
       </c>
       <c r="I81">
         <v>0.6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82">
+        <v>0.7</v>
+      </c>
+      <c r="C82">
+        <v>1234</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="E82" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82">
+        <v>1</v>
+      </c>
+      <c r="G82">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="H82">
+        <v>0.35920036204419398</v>
+      </c>
+      <c r="I82">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83">
+        <v>0.7</v>
+      </c>
+      <c r="C83">
+        <v>1234</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83">
+        <v>2</v>
+      </c>
+      <c r="G83">
+        <v>0.59523809523809501</v>
+      </c>
+      <c r="H83">
+        <v>0.35196828851129802</v>
+      </c>
+      <c r="I83">
+        <v>0.45833333333333298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84">
+        <v>0.7</v>
+      </c>
+      <c r="C84">
+        <v>1234</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84">
+        <v>3</v>
+      </c>
+      <c r="G84">
+        <v>0.51428571428571401</v>
+      </c>
+      <c r="H84">
+        <v>0.40329853998743398</v>
+      </c>
+      <c r="I84">
+        <v>0.41666666666666602</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85">
+        <v>0.7</v>
+      </c>
+      <c r="C85">
+        <v>1234</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85">
+        <v>4</v>
+      </c>
+      <c r="G85">
+        <v>0.48</v>
+      </c>
+      <c r="H85">
+        <v>0.41937749732716301</v>
+      </c>
+      <c r="I85">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86">
+        <v>0.7</v>
+      </c>
+      <c r="C86">
+        <v>1234</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="E86" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86">
+        <v>5</v>
+      </c>
+      <c r="G86">
+        <v>0.61285714285714199</v>
+      </c>
+      <c r="H86">
+        <v>0.368190734559739</v>
+      </c>
+      <c r="I86">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87">
+        <v>0.7</v>
+      </c>
+      <c r="C87">
+        <v>1234</v>
+      </c>
+      <c r="D87">
+        <v>3</v>
+      </c>
+      <c r="E87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F87">
+        <v>6</v>
+      </c>
+      <c r="G87">
+        <v>0.56666666666666599</v>
+      </c>
+      <c r="H87">
+        <v>0.36663896644976302</v>
+      </c>
+      <c r="I87">
+        <v>0.45833333333333298</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88">
+        <v>0.7</v>
+      </c>
+      <c r="C88">
+        <v>1234</v>
+      </c>
+      <c r="D88">
+        <v>3</v>
+      </c>
+      <c r="E88" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88">
+        <v>7</v>
+      </c>
+      <c r="G88">
+        <v>0.53095238095238095</v>
+      </c>
+      <c r="H88">
+        <v>0.42054538283457898</v>
+      </c>
+      <c r="I88">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89">
+        <v>0.7</v>
+      </c>
+      <c r="C89">
+        <v>1234</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="E89" t="s">
+        <v>10</v>
+      </c>
+      <c r="F89">
+        <v>8</v>
+      </c>
+      <c r="G89">
+        <v>0.59809523809523801</v>
+      </c>
+      <c r="H89">
+        <v>0.36231760915803701</v>
+      </c>
+      <c r="I89">
+        <v>0.41666666666666602</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90">
+        <v>0.7</v>
+      </c>
+      <c r="C90">
+        <v>1234</v>
+      </c>
+      <c r="D90">
+        <v>3</v>
+      </c>
+      <c r="E90" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90">
+        <v>9</v>
+      </c>
+      <c r="G90">
+        <v>0.51619047619047598</v>
+      </c>
+      <c r="H90">
+        <v>0.373460047833166</v>
+      </c>
+      <c r="I90">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91">
+        <v>0.7</v>
+      </c>
+      <c r="C91">
+        <v>1234</v>
+      </c>
+      <c r="D91">
+        <v>3</v>
+      </c>
+      <c r="E91" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91">
+        <v>10</v>
+      </c>
+      <c r="G91">
+        <v>0.48380952380952302</v>
+      </c>
+      <c r="H91">
+        <v>0.39312151855162197</v>
+      </c>
+      <c r="I91">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>8</v>
+      </c>
+      <c r="B92">
+        <v>0.8</v>
+      </c>
+      <c r="C92">
+        <v>1234</v>
+      </c>
+      <c r="D92">
+        <v>3</v>
+      </c>
+      <c r="E92" t="s">
+        <v>10</v>
+      </c>
+      <c r="F92">
+        <v>1</v>
+      </c>
+      <c r="G92">
+        <v>0.60595238095238002</v>
+      </c>
+      <c r="H92">
+        <v>0.360257777881972</v>
+      </c>
+      <c r="I92">
+        <v>0.28571428571428498</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>8</v>
+      </c>
+      <c r="B93">
+        <v>0.8</v>
+      </c>
+      <c r="C93">
+        <v>1234</v>
+      </c>
+      <c r="D93">
+        <v>3</v>
+      </c>
+      <c r="E93" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93">
+        <v>2</v>
+      </c>
+      <c r="G93">
+        <v>0.52222222222222203</v>
+      </c>
+      <c r="H93">
+        <v>0.38530449680178303</v>
+      </c>
+      <c r="I93">
+        <v>0.57142857142857095</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>8</v>
+      </c>
+      <c r="B94">
+        <v>0.8</v>
+      </c>
+      <c r="C94">
+        <v>1234</v>
+      </c>
+      <c r="D94">
+        <v>3</v>
+      </c>
+      <c r="E94" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94">
+        <v>3</v>
+      </c>
+      <c r="G94">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="H94">
+        <v>0.39497721450861201</v>
+      </c>
+      <c r="I94">
+        <v>0.57142857142857095</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95">
+        <v>0.8</v>
+      </c>
+      <c r="C95">
+        <v>1234</v>
+      </c>
+      <c r="D95">
+        <v>3</v>
+      </c>
+      <c r="E95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95">
+        <v>4</v>
+      </c>
+      <c r="G95">
+        <v>0.59285714285714197</v>
+      </c>
+      <c r="H95">
+        <v>0.37065369935043802</v>
+      </c>
+      <c r="I95">
+        <v>0.42857142857142799</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96">
+        <v>0.8</v>
+      </c>
+      <c r="C96">
+        <v>1234</v>
+      </c>
+      <c r="D96">
+        <v>3</v>
+      </c>
+      <c r="E96" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96">
+        <v>5</v>
+      </c>
+      <c r="G96">
+        <v>0.525595238095238</v>
+      </c>
+      <c r="H96">
+        <v>0.39785222849909302</v>
+      </c>
+      <c r="I96">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>8</v>
+      </c>
+      <c r="B97">
+        <v>0.8</v>
+      </c>
+      <c r="C97">
+        <v>1234</v>
+      </c>
+      <c r="D97">
+        <v>3</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97">
+        <v>6</v>
+      </c>
+      <c r="G97">
+        <v>0.46071428571428502</v>
+      </c>
+      <c r="H97">
+        <v>0.38028707332199402</v>
+      </c>
+      <c r="I97">
+        <v>0.57142857142857095</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98">
+        <v>0.8</v>
+      </c>
+      <c r="C98">
+        <v>1234</v>
+      </c>
+      <c r="D98">
+        <v>3</v>
+      </c>
+      <c r="E98" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98">
+        <v>7</v>
+      </c>
+      <c r="G98">
+        <v>0.48690476190476101</v>
+      </c>
+      <c r="H98">
+        <v>0.39852929217598898</v>
+      </c>
+      <c r="I98">
+        <v>0.64285714285714202</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99">
+        <v>0.8</v>
+      </c>
+      <c r="C99">
+        <v>1234</v>
+      </c>
+      <c r="D99">
+        <v>3</v>
+      </c>
+      <c r="E99" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99">
+        <v>8</v>
+      </c>
+      <c r="G99">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H99">
+        <v>0.40308755491190901</v>
+      </c>
+      <c r="I99">
+        <v>0.64285714285714202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100">
+        <v>0.8</v>
+      </c>
+      <c r="C100">
+        <v>1234</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
+      <c r="E100" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100">
+        <v>9</v>
+      </c>
+      <c r="G100">
+        <v>0.54087301587301495</v>
+      </c>
+      <c r="H100">
+        <v>0.40507618263550599</v>
+      </c>
+      <c r="I100">
+        <v>0.57142857142857095</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>8</v>
+      </c>
+      <c r="B101">
+        <v>0.8</v>
+      </c>
+      <c r="C101">
+        <v>1234</v>
+      </c>
+      <c r="D101">
+        <v>3</v>
+      </c>
+      <c r="E101" t="s">
+        <v>10</v>
+      </c>
+      <c r="F101">
+        <v>10</v>
+      </c>
+      <c r="G101">
+        <v>0.46666666666666601</v>
+      </c>
+      <c r="H101">
+        <v>0.417760934199435</v>
+      </c>
+      <c r="I101">
+        <v>0.57142857142857095</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102">
+        <v>0.7</v>
+      </c>
+      <c r="C102">
+        <v>1234</v>
+      </c>
+      <c r="D102">
+        <v>2</v>
+      </c>
+      <c r="E102" t="s">
+        <v>10</v>
+      </c>
+      <c r="F102">
+        <v>1</v>
+      </c>
+      <c r="G102">
+        <v>0.79666666666666597</v>
+      </c>
+      <c r="H102">
+        <v>0.15564609705922899</v>
+      </c>
+      <c r="I102">
+        <v>0.73333333333333295</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103">
+        <v>0.7</v>
+      </c>
+      <c r="C103">
+        <v>1234</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
+      </c>
+      <c r="E103" t="s">
+        <v>10</v>
+      </c>
+      <c r="F103">
+        <v>2</v>
+      </c>
+      <c r="G103">
+        <v>0.71833333333333305</v>
+      </c>
+      <c r="H103">
+        <v>0.16902623806633399</v>
+      </c>
+      <c r="I103">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104">
+        <v>0.7</v>
+      </c>
+      <c r="C104">
+        <v>1234</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
+      <c r="E104" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104">
+        <v>3</v>
+      </c>
+      <c r="G104">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="H104">
+        <v>0.23366942709202099</v>
+      </c>
+      <c r="I104">
+        <v>0.73333333333333295</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105">
+        <v>0.7</v>
+      </c>
+      <c r="C105">
+        <v>1234</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
+      </c>
+      <c r="E105" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105">
+        <v>4</v>
+      </c>
+      <c r="G105">
+        <v>0.68166666666666598</v>
+      </c>
+      <c r="H105">
+        <v>0.24509181212450601</v>
+      </c>
+      <c r="I105">
+        <v>0.86666666666666603</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>8</v>
+      </c>
+      <c r="B106">
+        <v>0.7</v>
+      </c>
+      <c r="C106">
+        <v>1234</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+      <c r="E106" t="s">
+        <v>10</v>
+      </c>
+      <c r="F106">
+        <v>5</v>
+      </c>
+      <c r="G106">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="H106">
+        <v>0.15643755966498701</v>
+      </c>
+      <c r="I106">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107">
+        <v>0.7</v>
+      </c>
+      <c r="C107">
+        <v>1234</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+      <c r="E107" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107">
+        <v>6</v>
+      </c>
+      <c r="G107">
+        <v>0.83</v>
+      </c>
+      <c r="H107">
+        <v>0.14982702234190701</v>
+      </c>
+      <c r="I107">
+        <v>0.53333333333333299</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>8</v>
+      </c>
+      <c r="B108">
+        <v>0.7</v>
+      </c>
+      <c r="C108">
+        <v>1234</v>
+      </c>
+      <c r="D108">
+        <v>2</v>
+      </c>
+      <c r="E108" t="s">
+        <v>10</v>
+      </c>
+      <c r="F108">
+        <v>7</v>
+      </c>
+      <c r="G108">
+        <v>0.71833333333333305</v>
+      </c>
+      <c r="H108">
+        <v>0.197329652703748</v>
+      </c>
+      <c r="I108">
+        <v>0.73333333333333295</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>8</v>
+      </c>
+      <c r="B109">
+        <v>0.7</v>
+      </c>
+      <c r="C109">
+        <v>1234</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
+      </c>
+      <c r="E109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F109">
+        <v>8</v>
+      </c>
+      <c r="G109">
+        <v>0.76666666666666605</v>
+      </c>
+      <c r="H109">
+        <v>0.16529929171822999</v>
+      </c>
+      <c r="I109">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>8</v>
+      </c>
+      <c r="B110">
+        <v>0.7</v>
+      </c>
+      <c r="C110">
+        <v>1234</v>
+      </c>
+      <c r="D110">
+        <v>2</v>
+      </c>
+      <c r="E110" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110">
+        <v>9</v>
+      </c>
+      <c r="G110">
+        <v>0.65666666666666595</v>
+      </c>
+      <c r="H110">
+        <v>0.21598115424838901</v>
+      </c>
+      <c r="I110">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111">
+        <v>0.7</v>
+      </c>
+      <c r="C111">
+        <v>1234</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
+      <c r="E111" t="s">
+        <v>10</v>
+      </c>
+      <c r="F111">
+        <v>10</v>
+      </c>
+      <c r="G111">
+        <v>0.82166666666666599</v>
+      </c>
+      <c r="H111">
+        <v>0.14332613750804199</v>
+      </c>
+      <c r="I111">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112">
+        <v>0.8</v>
+      </c>
+      <c r="C112">
+        <v>1234</v>
+      </c>
+      <c r="D112">
+        <v>2</v>
+      </c>
+      <c r="E112" t="s">
+        <v>10</v>
+      </c>
+      <c r="F112">
+        <v>1</v>
+      </c>
+      <c r="G112">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="H112">
+        <v>0.16115501520387801</v>
+      </c>
+      <c r="I112">
+        <v>0.55555555555555503</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113">
+        <v>0.8</v>
+      </c>
+      <c r="C113">
+        <v>1234</v>
+      </c>
+      <c r="D113">
+        <v>2</v>
+      </c>
+      <c r="E113" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113">
+        <v>2</v>
+      </c>
+      <c r="G113">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="H113">
+        <v>0.18429886354876901</v>
+      </c>
+      <c r="I113">
+        <v>0.77777777777777701</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>8</v>
+      </c>
+      <c r="B114">
+        <v>0.8</v>
+      </c>
+      <c r="C114">
+        <v>1234</v>
+      </c>
+      <c r="D114">
+        <v>2</v>
+      </c>
+      <c r="E114" t="s">
+        <v>10</v>
+      </c>
+      <c r="F114">
+        <v>3</v>
+      </c>
+      <c r="G114">
+        <v>0.788333333333333</v>
+      </c>
+      <c r="H114">
+        <v>0.15816544173355901</v>
+      </c>
+      <c r="I114">
+        <v>0.55555555555555503</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115">
+        <v>0.8</v>
+      </c>
+      <c r="C115">
+        <v>1234</v>
+      </c>
+      <c r="D115">
+        <v>2</v>
+      </c>
+      <c r="E115" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115">
+        <v>4</v>
+      </c>
+      <c r="G115">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="H115">
+        <v>0.18628141973692899</v>
+      </c>
+      <c r="I115">
+        <v>0.66666666666666596</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116">
+        <v>0.8</v>
+      </c>
+      <c r="C116">
+        <v>1234</v>
+      </c>
+      <c r="D116">
+        <v>2</v>
+      </c>
+      <c r="E116" t="s">
+        <v>10</v>
+      </c>
+      <c r="F116">
+        <v>5</v>
+      </c>
+      <c r="G116">
+        <v>0.69833333333333303</v>
+      </c>
+      <c r="H116">
+        <v>0.19849029259957299</v>
+      </c>
+      <c r="I116">
+        <v>0.77777777777777701</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>8</v>
+      </c>
+      <c r="B117">
+        <v>0.8</v>
+      </c>
+      <c r="C117">
+        <v>1234</v>
+      </c>
+      <c r="D117">
+        <v>2</v>
+      </c>
+      <c r="E117" t="s">
+        <v>10</v>
+      </c>
+      <c r="F117">
+        <v>6</v>
+      </c>
+      <c r="G117">
+        <v>0.79</v>
+      </c>
+      <c r="H117">
+        <v>0.171673746108428</v>
+      </c>
+      <c r="I117">
+        <v>0.55555555555555503</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>8</v>
+      </c>
+      <c r="B118">
+        <v>0.8</v>
+      </c>
+      <c r="C118">
+        <v>1234</v>
+      </c>
+      <c r="D118">
+        <v>2</v>
+      </c>
+      <c r="E118" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118">
+        <v>7</v>
+      </c>
+      <c r="G118">
+        <v>0.73</v>
+      </c>
+      <c r="H118">
+        <v>0.18660867754823099</v>
+      </c>
+      <c r="I118">
+        <v>0.77777777777777701</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119">
+        <v>0.8</v>
+      </c>
+      <c r="C119">
+        <v>1234</v>
+      </c>
+      <c r="D119">
+        <v>2</v>
+      </c>
+      <c r="E119" t="s">
+        <v>10</v>
+      </c>
+      <c r="F119">
+        <v>8</v>
+      </c>
+      <c r="G119">
+        <v>0.71</v>
+      </c>
+      <c r="H119">
+        <v>0.205384611843589</v>
+      </c>
+      <c r="I119">
+        <v>0.88888888888888795</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>8</v>
+      </c>
+      <c r="B120">
+        <v>0.8</v>
+      </c>
+      <c r="C120">
+        <v>1234</v>
+      </c>
+      <c r="D120">
+        <v>2</v>
+      </c>
+      <c r="E120" t="s">
+        <v>10</v>
+      </c>
+      <c r="F120">
+        <v>9</v>
+      </c>
+      <c r="G120">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H120">
+        <v>0.184019130568876</v>
+      </c>
+      <c r="I120">
+        <v>0.77777777777777701</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>8</v>
+      </c>
+      <c r="B121">
+        <v>0.8</v>
+      </c>
+      <c r="C121">
+        <v>1234</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
+      </c>
+      <c r="E121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121">
+        <v>10</v>
+      </c>
+      <c r="G121">
+        <v>0.65833333333333299</v>
+      </c>
+      <c r="H121">
+        <v>0.20893617351920099</v>
+      </c>
+      <c r="I121">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>